<commit_message>
extend design sheet by other classes and methods (a2c, controller, MultiAgentController, RankLearner)
</commit_message>
<xml_diff>
--- a/requirements/Design_Sheet.xlsx
+++ b/requirements/Design_Sheet.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\GitHub\robust-marl4sas\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krah/eclipse-workspace/robust-marl4sas/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBC8B44-C22F-4169-9FCD-CFF5C8468F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDDAB35-088E-694E-9AC7-61F67F524A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="18413" windowHeight="10996" xr2:uid="{B6EFE1A8-0685-4C11-A449-D6DF880E3A3E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22420" activeTab="3" xr2:uid="{B6EFE1A8-0685-4C11-A449-D6DF880E3A3E}"/>
   </bookViews>
   <sheets>
     <sheet name="BrokenComponents.py" sheetId="1" r:id="rId1"/>
+    <sheet name="Agent.py" sheetId="2" r:id="rId2"/>
+    <sheet name="MultiAgentController.py" sheetId="3" r:id="rId3"/>
+    <sheet name="RankLearner.py" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="132">
   <si>
     <t>__init__</t>
   </si>
@@ -151,12 +154,419 @@
     <t xml:space="preserve">Currently initializes the state space, various hyperparameters to determine stochasticity of rewards
 </t>
   </si>
+  <si>
+    <t>Currently initializes the state space, various hyperparameters of the model</t>
+  </si>
+  <si>
+    <t>no change</t>
+  </si>
+  <si>
+    <t>train_by_batches</t>
+  </si>
+  <si>
+    <t>train_by_episodes</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>_returns_advantages</t>
+  </si>
+  <si>
+    <t>_value_loss</t>
+  </si>
+  <si>
+    <t>_logits_loss</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">A2CAgent: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Encapsulate the model so it can be replaced easily with another algorithm. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">MultiAgentController: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Will be used to coordinate the agents for centralized training and centralized ranking of decentralized executed search.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RankLearner: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Will learn to rank individual results of each agent</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Modification of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>algorithms.py</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Modification of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rl-4-self-repair/algorithm_analysis/a2c.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mrubis_controller/controller.py</t>
+    </r>
+  </si>
+  <si>
+    <t>a2c.py</t>
+  </si>
+  <si>
+    <t>controller.py</t>
+  </si>
+  <si>
+    <t>desired interface:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trains n numbers of updates (default 250) in batches on the Environment env. </t>
+  </si>
+  <si>
+    <t>calculates the advantages of the next_values by using the rewards, dones, values and next_value</t>
+  </si>
+  <si>
+    <t>Value loss is typically MSE between value estimates and returns.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        # A trick to input actions and advantages through the same API.</t>
+  </si>
+  <si>
+    <t>Should be moved into the model and handled as in input there so the model implementation could be exchanged. Alternatively this could stay the same, if the whole agent is replaced rather then just the model jused internally.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evalutes one episode on the env and returns the cumulative reward </t>
+  </si>
+  <si>
+    <t>as the environment is not included in this agent anymore, the method will be changed to work without a loop and without the env and will just get the input to calc the next action. The reward must be handled externally per agent</t>
+  </si>
+  <si>
+    <t>same as before but one a single batch only</t>
+  </si>
+  <si>
+    <t>same changes here as for train_by_batch</t>
+  </si>
+  <si>
+    <t>as the training will be moved to central instance, there is no individual training fo single agents planned</t>
+  </si>
+  <si>
+    <t>Create a new instance of the mRubisController class, starts connection to mRUBIS, sets hyperparameters</t>
+  </si>
+  <si>
+    <t>needs to be moved to the BrokenComponents.py</t>
+  </si>
+  <si>
+    <t>_start_mrubis</t>
+  </si>
+  <si>
+    <t>Launch mRUBiS as a subprocess. NOTE: Unstable. Manual startup from Eclipse is more robust.</t>
+  </si>
+  <si>
+    <t>needs to be moved to the BrokenComponents.py
++ stabilize implemementation</t>
+  </si>
+  <si>
+    <t>_connect_to_java</t>
+  </si>
+  <si>
+    <t>Connect to the socket opened on the java side</t>
+  </si>
+  <si>
+    <t>&gt;&gt; BrokenComponents.py</t>
+  </si>
+  <si>
+    <t>_get_initial_state</t>
+  </si>
+  <si>
+    <t>Query mRUBiS for the number of shops, get their initial states</t>
+  </si>
+  <si>
+    <t>_update_number_of_issues_in_run</t>
+  </si>
+  <si>
+    <t>Update the number of issues present in the current run</t>
+  </si>
+  <si>
+    <t>&gt;&gt; MultiAgentController.py</t>
+  </si>
+  <si>
+    <t>&gt;&gt; MultiAgentController.py
+each agent will be initialized with the corresponding state</t>
+  </si>
+  <si>
+    <t>QUESTIONS</t>
+  </si>
+  <si>
+    <t>Do we distribute the shops per agent randomly and evenly?</t>
+  </si>
+  <si>
+    <t>_get_from_mrubis</t>
+  </si>
+  <si>
+    <t>Send a message to mRUBiS and return the response as a dictionary</t>
+  </si>
+  <si>
+    <t>_get_info_from_issue</t>
+  </si>
+  <si>
+    <t>Parse relevant information out of an issue dictionary</t>
+  </si>
+  <si>
+    <t>_pick_rule</t>
+  </si>
+  <si>
+    <t>Pick a rule to apply to an issue using a strategy</t>
+  </si>
+  <si>
+    <t>not needed, as we use the a2c agent for this</t>
+  </si>
+  <si>
+    <t>_send_rule_to_execute</t>
+  </si>
+  <si>
+    <t>Send a rule to apply to an issue to mRUBiS</t>
+  </si>
+  <si>
+    <t>_predict_optimal_utility_of_fixed_components</t>
+  </si>
+  <si>
+    <t>Predict the optimal utility of a component which should be fixed</t>
+  </si>
+  <si>
+    <t>no change here, we will still use this in the agent for ranking internally in the agent</t>
+  </si>
+  <si>
+    <t>__get_ranked_fix_instructions</t>
+  </si>
+  <si>
+    <t>Get a list of tuples containing the fixes to apply ranked by a strategy</t>
+  </si>
+  <si>
+    <t>_get_component_fixing_order</t>
+  </si>
+  <si>
+    <t>Not used anymore as we're using the a2c for selection a fix (and there is only one fix avabilabe…)</t>
+  </si>
+  <si>
+    <t>Get a complete list of all components to fix ranked by a ranking strategy</t>
+  </si>
+  <si>
+    <t>_cumulative_utility_based_on_order</t>
+  </si>
+  <si>
+    <t>as method says</t>
+  </si>
+  <si>
+    <t>_send_order_in_which_to_apply_fixes</t>
+  </si>
+  <si>
+    <t>Send the order in which to apply the fixes to mRUBiS</t>
+  </si>
+  <si>
+    <t>_send_exit_message</t>
+  </si>
+  <si>
+    <t>_close_socket</t>
+  </si>
+  <si>
+    <t>_state_to_df</t>
+  </si>
+  <si>
+    <t>_set_shop_and_system_utility</t>
+  </si>
+  <si>
+    <t>Make the shop and system utility fields uniform across the run</t>
+  </si>
+  <si>
+    <t>_write_mrubis_state_history_to_disk</t>
+  </si>
+  <si>
+    <t>Write the state history to disk</t>
+  </si>
+  <si>
+    <t>_write_df_list_to_disk</t>
+  </si>
+  <si>
+    <t>_update_current_state</t>
+  </si>
+  <si>
+    <t>_reset_predicted_utility</t>
+  </si>
+  <si>
+    <t>_remove_replaced_authentication_service</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>__main__</t>
+  </si>
+  <si>
+    <t>Tell mRUBiS to stop its main loop</t>
+  </si>
+  <si>
+    <t>Close the socket</t>
+  </si>
+  <si>
+    <t>Return the current mRUBiS state as a pandas dataframe</t>
+  </si>
+  <si>
+    <t>Should be done in the MultiAgentController probably</t>
+  </si>
+  <si>
+    <t>logging</t>
+  </si>
+  <si>
+    <t>''Update the controller's current mRUBiS state with an incoming state'''
+        '''TODO: This is not a state, but a data update. '''</t>
+  </si>
+  <si>
+    <t>&gt;&gt; BrokenComponents.py
+update the environment and each agent as well</t>
+  </si>
+  <si>
+    <t>Reset the predicted utility field for components that have been fixed</t>
+  </si>
+  <si>
+    <t>Will probably not be used anymore in the agent and can be removed. But depends on the implementation of the agent</t>
+  </si>
+  <si>
+    <t>Remove instances of the Authentication Service component that have been replaced</t>
+  </si>
+  <si>
+    <t>Check if this is needed?</t>
+  </si>
+  <si>
+    <t>Run and control mRUBiS for a maximum number of runs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt; MultiAgentController.py
+</t>
+  </si>
+  <si>
+    <t>starts the controller</t>
+  </si>
+  <si>
+    <t>get_sorted_actions</t>
+  </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
+    <t>Should return the sorted fixed for the current internal action state or by passing observations relevant for the agent</t>
+  </si>
+  <si>
+    <t>update the agents models network parameters to improve the next sorting</t>
+  </si>
+  <si>
+    <t>desired interface</t>
+  </si>
+  <si>
+    <t>init all agents and init env</t>
+  </si>
+  <si>
+    <t xml:space="preserve">init env connection and start training loop with all agents and the rank learner and communicate rewards </t>
+  </si>
+  <si>
+    <t>method to test the current agents against the env</t>
+  </si>
+  <si>
+    <t>test (get_ranking)</t>
+  </si>
+  <si>
+    <t>Calculate the ranking from the current input (either q-values, sorted lists, observations, …)</t>
+  </si>
+  <si>
+    <t>Improve ranking while training</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,16 +582,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -189,11 +620,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -204,11 +655,117 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="25">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -238,12 +795,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A273850-DA8F-40FD-A8F9-5485FD6DC179}" name="Table1" displayName="Table1" ref="B4:D13" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A273850-DA8F-40FD-A8F9-5485FD6DC179}" name="Table1" displayName="Table1" ref="B4:D13" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="B4:D13" xr:uid="{5A273850-DA8F-40FD-A8F9-5485FD6DC179}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{79412530-C358-4669-AF6E-0F03B8879991}" name="Functions" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{D68F9B25-82CA-4396-AFC4-F9ACEB9D2A25}" name="AS-IS" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{4941EB00-D9B8-47E1-BDD6-239434DDE106}" name="TO-BE" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{79412530-C358-4669-AF6E-0F03B8879991}" name="Functions" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{D68F9B25-82CA-4396-AFC4-F9ACEB9D2A25}" name="AS-IS" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{4941EB00-D9B8-47E1-BDD6-239434DDE106}" name="TO-BE" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{94F07DCE-194B-7449-B599-46281164AA96}" name="Table13" displayName="Table13" ref="B5:D14" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="B5:D14" xr:uid="{94F07DCE-194B-7449-B599-46281164AA96}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{D689ABAE-C123-8F47-8852-7EC472E01216}" name="Functions" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{359BEE40-ADC9-1840-9CED-866D42198E7F}" name="AS-IS" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{46572348-A5A7-3D46-B030-BE517C3744C4}" name="TO-BE" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A5F6E179-2E2F-0743-AD64-DA0FAAABD0EF}" name="Table135" displayName="Table135" ref="B17:D43" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B17:D43" xr:uid="{A5F6E179-2E2F-0743-AD64-DA0FAAABD0EF}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{BBF96C5D-BE99-4546-9B65-8F224BDFA0D3}" name="Functions" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{63EF920C-F08C-1941-B4C1-9B4E00BD77F6}" name="AS-IS" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{542D6672-BC07-0045-98F5-8404BF57FF8A}" name="TO-BE" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EDD74231-86EF-ED43-B011-63A6AF43BA1F}" name="Table136" displayName="Table136" ref="B46:D49" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="B46:D49" xr:uid="{EDD74231-86EF-ED43-B011-63A6AF43BA1F}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{EC841690-947E-C44C-93D8-A184A6CCD9CE}" name="Functions" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{0647137D-65A7-704B-8D6A-5CB518CFD6FD}" name="AS-IS" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{B86834C7-0CE6-BA44-96D9-45BC1C734740}" name="TO-BE" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{50FBA1DE-8B33-0D4D-A90D-54D9478868AB}" name="Table134" displayName="Table134" ref="B3:D12" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="B3:D12" xr:uid="{50FBA1DE-8B33-0D4D-A90D-54D9478868AB}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0AE47785-C1C5-AF44-B169-06A9933C16D4}" name="Functions" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{6C6AEC68-68EB-5F46-BFD9-B718499AC5A0}" name="AS-IS" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{F07A71CD-F2A0-6D4E-85C3-EBB9B2B68DED}" name="TO-BE" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -548,26 +1153,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5D2FB1-03C2-426F-92EA-9EE57ADE0D2F}">
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.3984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="48.86328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="48.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24.9296875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.06640625" style="1"/>
+    <col min="5" max="5" width="25" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="128.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" ht="144" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
@@ -578,7 +1183,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,7 +1194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
@@ -600,7 +1205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
@@ -611,7 +1216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
@@ -622,7 +1227,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
@@ -633,7 +1238,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
@@ -644,7 +1249,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
@@ -655,7 +1260,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
@@ -666,7 +1271,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
@@ -684,4 +1289,872 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD400633-0A89-F04D-80D1-6A880815203E}">
+  <dimension ref="A1:F55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B45" sqref="B45:D45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="4" max="4" width="61.33203125" customWidth="1"/>
+    <col min="6" max="6" width="45" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+    </row>
+    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B45:D45"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC24EBFD-5571-FC42-9342-2AB78061BE87}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="51.6640625" customWidth="1"/>
+    <col min="4" max="4" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD071AA-27B7-8F4C-9899-48A519D31A33}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="4" max="4" width="57.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>